<commit_message>
A whole bunch of Changes since last
</commit_message>
<xml_diff>
--- a/Distribution calcs.xlsx
+++ b/Distribution calcs.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/35c41b01ebcf9830/Documents/PhD_Storage/NAEI/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F3FF2AF-0129-49D3-9E7E-B2D489C8584D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="naei_ukdata_20210113102859" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">naei_ukdata_20210113102859!$A$2:$I$295</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
     <pivotCache cacheId="1" r:id="rId6"/>
@@ -886,7 +880,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1447,7 +1441,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Blyth, Liam" refreshedDate="44209.443067939814" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="293" xr:uid="{00000000-000A-0000-FFFF-FFFF06000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Blyth, Liam" refreshedDate="44209.443067939814" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="293">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:G295" sheet="naei_ukdata_20210113102859"/>
   </cacheSource>
@@ -1611,7 +1605,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Blyth, Liam" refreshedDate="44209.473294212963" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="55" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Blyth, Liam" refreshedDate="44209.473294212963" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="55">
   <cacheSource type="worksheet">
     <worksheetSource ref="H3:J58" sheet="Distribution calcs"/>
   </cacheSource>
@@ -4276,7 +4270,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B78" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -4622,7 +4616,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L4:M15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -4743,7 +4737,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4776,26 +4770,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4828,23 +4805,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5020,11 +4980,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I295"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J295"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5411,11 +5371,11 @@
       </c>
       <c r="H13">
         <f>VLOOKUP(E13,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>10</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="0"/>
-        <v>-103.52758585388399</v>
+        <v>1.03527585853884</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -5539,11 +5499,11 @@
       </c>
       <c r="H17">
         <f>VLOOKUP(E17,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" si="0"/>
-        <v>-35.504278448647788</v>
+        <v>22.905986095901799</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -5571,11 +5531,11 @@
       </c>
       <c r="H18">
         <f>VLOOKUP(E18,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>56.3</v>
+        <v>100</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" si="0"/>
-        <v>516.93129456716179</v>
+        <v>918.1728145065041</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -5827,11 +5787,11 @@
       </c>
       <c r="H26">
         <f>VLOOKUP(E26,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>10</v>
       </c>
       <c r="I26" s="5">
         <f t="shared" si="0"/>
-        <v>-25.410804664251298</v>
+        <v>0.25410804664251296</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -5859,11 +5819,11 @@
       </c>
       <c r="H27">
         <f>VLOOKUP(E27,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I27" s="5">
         <f t="shared" si="0"/>
-        <v>-216.73222005415357</v>
+        <v>139.82723874461522</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -6114,7 +6074,7 @@
       </c>
       <c r="H35">
         <f>VLOOKUP(E35,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I35" s="5">
         <f t="shared" si="0"/>
@@ -8130,11 +8090,11 @@
       </c>
       <c r="H98">
         <f>VLOOKUP(E98,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I98" s="5">
         <f t="shared" si="1"/>
-        <v>-5138.6367430625005</v>
+        <v>-4876.5662691663128</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -8194,11 +8154,11 @@
       </c>
       <c r="H100">
         <f>VLOOKUP(E100,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I100" s="5">
         <f t="shared" si="1"/>
-        <v>-217962.68373942899</v>
+        <v>-206846.58686871812</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -8642,11 +8602,11 @@
       </c>
       <c r="H114">
         <f>VLOOKUP(E114,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>56.3</v>
+        <v>100</v>
       </c>
       <c r="I114" s="5">
         <f t="shared" si="1"/>
-        <v>403.632671523</v>
+        <v>716.93192099999999</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -8706,11 +8666,11 @@
       </c>
       <c r="H116">
         <f>VLOOKUP(E116,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I116" s="5">
         <f t="shared" si="1"/>
-        <v>-1134.3128326904466</v>
+        <v>731.81473076803002</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -9058,11 +9018,11 @@
       </c>
       <c r="H127">
         <f>VLOOKUP(E127,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I127" s="5">
         <f t="shared" si="1"/>
-        <v>-44391.965966493102</v>
+        <v>-42127.975702201955</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -9090,11 +9050,11 @@
       </c>
       <c r="H128">
         <f>VLOOKUP(E128,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I128" s="5">
         <f t="shared" si="1"/>
-        <v>-3208.4818980372297</v>
+        <v>-3044.849321237331</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -9122,11 +9082,11 @@
       </c>
       <c r="H129">
         <f>VLOOKUP(E129,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I129" s="5">
         <f t="shared" si="1"/>
-        <v>-34715.197650583796</v>
+        <v>-32944.722570404025</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -9154,11 +9114,11 @@
       </c>
       <c r="H130">
         <f>VLOOKUP(E130,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I130" s="5">
         <f t="shared" si="1"/>
-        <v>-4980.7197239161196</v>
+        <v>-4726.7030179963976</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -9186,11 +9146,11 @@
       </c>
       <c r="H131">
         <f>VLOOKUP(E131,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I131" s="5">
         <f t="shared" si="1"/>
-        <v>-22432.548551392301</v>
+        <v>-21288.488575271294</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -9218,11 +9178,11 @@
       </c>
       <c r="H132">
         <f>VLOOKUP(E132,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I132" s="5">
         <f t="shared" ref="I132:I195" si="2">G132*H132</f>
-        <v>-1559.6371437533201</v>
+        <v>-1480.0956494219008</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -9250,11 +9210,11 @@
       </c>
       <c r="H133">
         <f>VLOOKUP(E133,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I133" s="5">
         <f t="shared" si="2"/>
-        <v>-66511.8116350989</v>
+        <v>-63119.70924170885</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -9282,11 +9242,11 @@
       </c>
       <c r="H134">
         <f>VLOOKUP(E134,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I134" s="5">
         <f t="shared" si="2"/>
-        <v>-1914.0249763664801</v>
+        <v>-1816.4097025717895</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -9314,11 +9274,11 @@
       </c>
       <c r="H135">
         <f>VLOOKUP(E135,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I135" s="5">
         <f t="shared" si="2"/>
-        <v>-1005.3444372620199</v>
+        <v>-954.07187096165694</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -9346,11 +9306,11 @@
       </c>
       <c r="H136">
         <f>VLOOKUP(E136,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I136" s="5">
         <f t="shared" si="2"/>
-        <v>-3234.50158906972</v>
+        <v>-3069.5420080271642</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -9378,11 +9338,11 @@
       </c>
       <c r="H137">
         <f>VLOOKUP(E137,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I137" s="5">
         <f t="shared" si="2"/>
-        <v>-1077.7676671131001</v>
+        <v>-1022.8015160903319</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -9410,11 +9370,11 @@
       </c>
       <c r="H138">
         <f>VLOOKUP(E138,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I138" s="5">
         <f t="shared" si="2"/>
-        <v>-2252.6825704446001</v>
+        <v>-2137.7957593519254</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -9442,11 +9402,11 @@
       </c>
       <c r="H139">
         <f>VLOOKUP(E139,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I139" s="5">
         <f t="shared" si="2"/>
-        <v>-895.91731048907502</v>
+        <v>-850.22552765413218</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -9474,11 +9434,11 @@
       </c>
       <c r="H140">
         <f>VLOOKUP(E140,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I140" s="5">
         <f t="shared" si="2"/>
-        <v>-1505.2895273265601</v>
+        <v>-1428.5197614329054</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -9506,11 +9466,11 @@
       </c>
       <c r="H141">
         <f>VLOOKUP(E141,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I141" s="5">
         <f t="shared" si="2"/>
-        <v>-1412.4186933696601</v>
+        <v>-1340.3853400078074</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -9538,11 +9498,11 @@
       </c>
       <c r="H142">
         <f>VLOOKUP(E142,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I142" s="5">
         <f t="shared" si="2"/>
-        <v>-1373.1872018760901</v>
+        <v>-1303.1546545804094</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -9570,11 +9530,11 @@
       </c>
       <c r="H143">
         <f>VLOOKUP(E143,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I143" s="5">
         <f t="shared" si="2"/>
-        <v>-578.11552641588105</v>
+        <v>-548.63163456867107</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -9602,11 +9562,11 @@
       </c>
       <c r="H144">
         <f>VLOOKUP(E144,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I144" s="5">
         <f t="shared" si="2"/>
-        <v>-1834.8612544108901</v>
+        <v>-1741.2833304359347</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -9634,11 +9594,11 @@
       </c>
       <c r="H145">
         <f>VLOOKUP(E145,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I145" s="5">
         <f t="shared" si="2"/>
-        <v>-2258.2427263996897</v>
+        <v>-2143.0723473533058</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -9666,11 +9626,11 @@
       </c>
       <c r="H146">
         <f>VLOOKUP(E146,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I146" s="5">
         <f t="shared" si="2"/>
-        <v>-2269.6082042070202</v>
+        <v>-2153.8581857924619</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -9698,11 +9658,11 @@
       </c>
       <c r="H147">
         <f>VLOOKUP(E147,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I147" s="5">
         <f t="shared" si="2"/>
-        <v>-474.44534829650695</v>
+        <v>-450.24863553338514</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -9730,11 +9690,11 @@
       </c>
       <c r="H148">
         <f>VLOOKUP(E148,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I148" s="5">
         <f t="shared" si="2"/>
-        <v>-1332.5230186118999</v>
+        <v>-1264.564344662693</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -9762,11 +9722,11 @@
       </c>
       <c r="H149">
         <f>VLOOKUP(E149,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I149" s="5">
         <f t="shared" si="2"/>
-        <v>-183.36427319243001</v>
+        <v>-174.01269525961607</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -9794,11 +9754,11 @@
       </c>
       <c r="H150">
         <f>VLOOKUP(E150,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I150" s="5">
         <f t="shared" si="2"/>
-        <v>-2584.2007523533402</v>
+        <v>-2452.4065139833197</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -9826,11 +9786,11 @@
       </c>
       <c r="H151">
         <f>VLOOKUP(E151,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I151" s="5">
         <f t="shared" si="2"/>
-        <v>-1363.92851134136</v>
+        <v>-1294.3681572629505</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -9858,7 +9818,7 @@
       </c>
       <c r="H152">
         <f>VLOOKUP(E152,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I152" s="5">
         <f t="shared" si="2"/>
@@ -9890,11 +9850,11 @@
       </c>
       <c r="H153">
         <f>VLOOKUP(E153,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I153" s="5">
         <f t="shared" si="2"/>
-        <v>-4503.6057780102792</v>
+        <v>-4273.9218833317555</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -9922,11 +9882,11 @@
       </c>
       <c r="H154">
         <f>VLOOKUP(E154,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I154" s="5">
         <f t="shared" si="2"/>
-        <v>-490.46915207314004</v>
+        <v>-465.45522531740988</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -9954,11 +9914,11 @@
       </c>
       <c r="H155">
         <f>VLOOKUP(E155,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I155" s="5">
         <f t="shared" si="2"/>
-        <v>-115.79586870380899</v>
+        <v>-109.89027939991473</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -9986,11 +9946,11 @@
       </c>
       <c r="H156">
         <f>VLOOKUP(E156,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I156" s="5">
         <f t="shared" si="2"/>
-        <v>-4236.5392253157897</v>
+        <v>-4020.4757248246842</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -10018,11 +9978,11 @@
       </c>
       <c r="H157">
         <f>VLOOKUP(E157,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I157" s="5">
         <f t="shared" si="2"/>
-        <v>-1030.06594810814</v>
+        <v>-977.53258475462485</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -10242,11 +10202,11 @@
       </c>
       <c r="H164">
         <f>VLOOKUP(E164,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I164" s="5">
         <f t="shared" si="2"/>
-        <v>-27.057509256555999</v>
+        <v>-25.677576284471645</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
@@ -10306,7 +10266,7 @@
       </c>
       <c r="H166">
         <f>VLOOKUP(E166,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I166" s="5">
         <f t="shared" si="2"/>
@@ -10338,11 +10298,11 @@
       </c>
       <c r="H167">
         <f>VLOOKUP(E167,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I167" s="5">
         <f t="shared" si="2"/>
-        <v>-1259.3271511795301</v>
+        <v>-1195.1014664693741</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -10402,11 +10362,11 @@
       </c>
       <c r="H169">
         <f>VLOOKUP(E169,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I169" s="5">
         <f t="shared" si="2"/>
-        <v>-20966.495867149501</v>
+        <v>-19897.204577924877</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -10434,7 +10394,7 @@
       </c>
       <c r="H170">
         <f>VLOOKUP(E170,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I170" s="5">
         <f t="shared" si="2"/>
@@ -10498,11 +10458,11 @@
       </c>
       <c r="H172">
         <f>VLOOKUP(E172,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I172" s="5">
         <f t="shared" si="2"/>
-        <v>-14024.958489317702</v>
+        <v>-13309.685606362498</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -10530,7 +10490,7 @@
       </c>
       <c r="H173">
         <f>VLOOKUP(E173,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I173" s="5">
         <f t="shared" si="2"/>
@@ -10594,7 +10554,7 @@
       </c>
       <c r="H175">
         <f>VLOOKUP(E175,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I175" s="5">
         <f t="shared" si="2"/>
@@ -10633,7 +10593,7 @@
         <v>-42.13490598165</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>5</v>
       </c>
@@ -10665,7 +10625,7 @@
         <v>-4.3596023330259301</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>5</v>
       </c>
@@ -10697,7 +10657,7 @@
         <v>-0.18084146963992698</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>5</v>
       </c>
@@ -10729,7 +10689,7 @@
         <v>-0.76894102079772098</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>5</v>
       </c>
@@ -10761,7 +10721,7 @@
         <v>-23.090145761610898</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>5</v>
       </c>
@@ -10793,7 +10753,7 @@
         <v>-2290.1766151114603</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>5</v>
       </c>
@@ -10825,7 +10785,7 @@
         <v>-295.58345413613301</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>5</v>
       </c>
@@ -10857,7 +10817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>5</v>
       </c>
@@ -10889,7 +10849,7 @@
         <v>-255.27849555119903</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>5</v>
       </c>
@@ -10921,7 +10881,7 @@
         <v>-151.64472882441902</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>5</v>
       </c>
@@ -10952,8 +10912,12 @@
         <f t="shared" si="2"/>
         <v>-5819.3651060177199</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J186">
+        <f>G186/SUMIF(C:C,C$186,G:G)</f>
+        <v>1.2632354957275745E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>5</v>
       </c>
@@ -10985,7 +10949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>5</v>
       </c>
@@ -11017,7 +10981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>5</v>
       </c>
@@ -11049,7 +11013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>5</v>
       </c>
@@ -11081,7 +11045,7 @@
         <v>-736.01991267244307</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>5</v>
       </c>
@@ -11113,7 +11077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>5</v>
       </c>
@@ -11145,7 +11109,7 @@
         <v>-111.69802536009</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>5</v>
       </c>
@@ -11177,7 +11141,7 @@
         <v>-99.048662670543294</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>5</v>
       </c>
@@ -11208,8 +11172,12 @@
         <f t="shared" si="2"/>
         <v>-3969.9286233852604</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J194">
+        <f>G194/SUMIF(C:C,C$186,G:G)</f>
+        <v>8.6177008336859214E-3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>5</v>
       </c>
@@ -11241,7 +11209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>5</v>
       </c>
@@ -11273,7 +11241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>5</v>
       </c>
@@ -11305,7 +11273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>5</v>
       </c>
@@ -11337,7 +11305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>5</v>
       </c>
@@ -11369,7 +11337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>5</v>
       </c>
@@ -11401,7 +11369,7 @@
         <v>-1.20409556230591</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>5</v>
       </c>
@@ -11433,7 +11401,7 @@
         <v>-10.5689696390764</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>5</v>
       </c>
@@ -11464,8 +11432,12 @@
         <f t="shared" si="3"/>
         <v>-30313.651753104699</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J202">
+        <f t="shared" ref="J202:J204" si="4">G202/SUMIF(C:C,C$186,G:G)</f>
+        <v>6.5803193650880831E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>5</v>
       </c>
@@ -11496,8 +11468,12 @@
         <f t="shared" si="3"/>
         <v>-4442.4321399596602</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J203">
+        <f t="shared" si="4"/>
+        <v>9.6433852565032067E-3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>5</v>
       </c>
@@ -11528,8 +11504,12 @@
         <f t="shared" si="3"/>
         <v>-45730.998961637299</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J204">
+        <f t="shared" si="4"/>
+        <v>9.9270315732008271E-2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>5</v>
       </c>
@@ -11561,7 +11541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>5</v>
       </c>
@@ -11593,7 +11573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>5</v>
       </c>
@@ -11625,7 +11605,7 @@
         <v>-360.59379556564403</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>5</v>
       </c>
@@ -11657,7 +11637,7 @@
         <v>-235.80128339850302</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>5</v>
       </c>
@@ -11688,8 +11668,12 @@
         <f t="shared" si="3"/>
         <v>-26115.795496693001</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J209">
+        <f t="shared" ref="J209:J211" si="5">G209/SUMIF(C:C,C$186,G:G)</f>
+        <v>5.6690720155142094E-2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>5</v>
       </c>
@@ -11720,8 +11704,12 @@
         <f t="shared" si="3"/>
         <v>-19493.588822462702</v>
       </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J210">
+        <f t="shared" si="5"/>
+        <v>4.2315601257238232E-2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>5</v>
       </c>
@@ -11752,8 +11740,12 @@
         <f t="shared" si="3"/>
         <v>-36223.366665522102</v>
       </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J211">
+        <f t="shared" si="5"/>
+        <v>7.8631674955957243E-2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>5</v>
       </c>
@@ -11785,7 +11777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>5</v>
       </c>
@@ -11810,14 +11802,18 @@
       </c>
       <c r="H213">
         <f>VLOOKUP(E213,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>56.3</v>
+        <v>100</v>
       </c>
       <c r="I213" s="5">
         <f t="shared" si="3"/>
-        <v>14872.81736608485</v>
-      </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26417.082355390499</v>
+      </c>
+      <c r="J213">
+        <f>G213/SUMIF(C:C,C$186,G:G)</f>
+        <v>0.57344736954860287</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>5</v>
       </c>
@@ -11842,14 +11838,14 @@
       </c>
       <c r="H214">
         <f>VLOOKUP(E214,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>59.25</v>
+        <v>115</v>
       </c>
       <c r="I214" s="5">
         <f t="shared" si="3"/>
-        <v>10.805172900566776</v>
-      </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20.972065545403868</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>5</v>
       </c>
@@ -11874,14 +11870,18 @@
       </c>
       <c r="H215">
         <f>VLOOKUP(E215,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I215" s="5">
         <f t="shared" si="3"/>
-        <v>-607.89284150000003</v>
-      </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+        <v>392.18893000000003</v>
+      </c>
+      <c r="J215">
+        <f>G215/SUMIF(C:C,C$186,G:G)</f>
+        <v>4.2567098676718464E-2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>5</v>
       </c>
@@ -11906,14 +11906,14 @@
       </c>
       <c r="H216">
         <f>VLOOKUP(E216,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I216" s="5">
         <f t="shared" si="3"/>
-        <v>-46.263716321234796</v>
-      </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-43.904266788851821</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>5</v>
       </c>
@@ -11938,14 +11938,14 @@
       </c>
       <c r="H217">
         <f>VLOOKUP(E217,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I217" s="5">
         <f t="shared" si="3"/>
-        <v>-72676.354329346199</v>
-      </c>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-68969.860258549539</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>5</v>
       </c>
@@ -11977,7 +11977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>5</v>
       </c>
@@ -12009,7 +12009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>5</v>
       </c>
@@ -12041,7 +12041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>5</v>
       </c>
@@ -12073,7 +12073,7 @@
         <v>-68.154727338360004</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>5</v>
       </c>
@@ -12105,7 +12105,7 @@
         <v>-98.252253006369301</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>5</v>
       </c>
@@ -12130,14 +12130,18 @@
       </c>
       <c r="H223">
         <f>VLOOKUP(E223,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I223" s="5">
         <f t="shared" si="3"/>
-        <v>-67.450568884666893</v>
-      </c>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43.516496054623801</v>
+      </c>
+      <c r="J223">
+        <f>G223/SUMIF(C:C,C$186,G:G)</f>
+        <v>4.7231597832763945E-3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>5</v>
       </c>
@@ -12226,11 +12230,11 @@
       </c>
       <c r="H226">
         <f>VLOOKUP(E226,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="I226" s="5">
         <f t="shared" si="3"/>
-        <v>-1076.64668456092</v>
+        <v>-1021.7377036483131</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -13154,11 +13158,11 @@
       </c>
       <c r="H255">
         <f>VLOOKUP(E255,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I255" s="5">
         <f t="shared" si="3"/>
-        <v>-56.433826945619039</v>
+        <v>36.408920610076798</v>
       </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
@@ -13317,7 +13321,7 @@
         <v>0</v>
       </c>
       <c r="I260" s="5">
-        <f t="shared" ref="I260:I295" si="4">G260*H260</f>
+        <f t="shared" ref="I260:I295" si="6">G260*H260</f>
         <v>0</v>
       </c>
     </row>
@@ -13349,7 +13353,7 @@
         <v>-1000</v>
       </c>
       <c r="I261" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -13381,7 +13385,7 @@
         <v>-1000</v>
       </c>
       <c r="I262" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-77.774925597275498</v>
       </c>
     </row>
@@ -13413,7 +13417,7 @@
         <v>-1000</v>
       </c>
       <c r="I263" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-138.02882317500001</v>
       </c>
     </row>
@@ -13445,7 +13449,7 @@
         <v>-1000</v>
       </c>
       <c r="I264" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1729.3505</v>
       </c>
     </row>
@@ -13477,7 +13481,7 @@
         <v>-1000</v>
       </c>
       <c r="I265" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-67.302760000000006</v>
       </c>
     </row>
@@ -13509,7 +13513,7 @@
         <v>-1000</v>
       </c>
       <c r="I266" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-3300</v>
       </c>
     </row>
@@ -13541,7 +13545,7 @@
         <v>0</v>
       </c>
       <c r="I267" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -13573,7 +13577,7 @@
         <v>0</v>
       </c>
       <c r="I268" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -13605,7 +13609,7 @@
         <v>0</v>
       </c>
       <c r="I269" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -13637,7 +13641,7 @@
         <v>0</v>
       </c>
       <c r="I270" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -13669,7 +13673,7 @@
         <v>0</v>
       </c>
       <c r="I271" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -13698,11 +13702,11 @@
       </c>
       <c r="H272">
         <f>VLOOKUP(E272,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>59.25</v>
+        <v>115</v>
       </c>
       <c r="I272" s="5">
-        <f t="shared" si="4"/>
-        <v>339.46981694964319</v>
+        <f t="shared" si="6"/>
+        <v>658.88656454361126</v>
       </c>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
@@ -13730,11 +13734,11 @@
       </c>
       <c r="H273">
         <f>VLOOKUP(E273,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="I273" s="5">
-        <f t="shared" si="4"/>
-        <v>17.404940088380005</v>
+        <f t="shared" si="6"/>
+        <v>40.05407327574995</v>
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
@@ -13762,11 +13766,11 @@
       </c>
       <c r="H274">
         <f>VLOOKUP(E274,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="I274" s="5">
-        <f t="shared" si="4"/>
-        <v>34.753190659854745</v>
+        <f t="shared" si="6"/>
+        <v>79.977686690531684</v>
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
@@ -13794,11 +13798,11 @@
       </c>
       <c r="H275">
         <f>VLOOKUP(E275,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="I275" s="5">
-        <f t="shared" si="4"/>
-        <v>27.849793771070665</v>
+        <f t="shared" si="6"/>
+        <v>64.090865855132961</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
@@ -13826,11 +13830,11 @@
       </c>
       <c r="H276">
         <f>VLOOKUP(E276,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="I276" s="5">
-        <f t="shared" si="4"/>
-        <v>285.21219000000002</v>
+        <f t="shared" si="6"/>
+        <v>656.36020000000008</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
@@ -13858,11 +13862,11 @@
       </c>
       <c r="H277">
         <f>VLOOKUP(E277,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I277" s="5">
-        <f t="shared" si="4"/>
-        <v>-84.602394416557303</v>
+        <f t="shared" si="6"/>
+        <v>54.582189946166004</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
@@ -13890,10 +13894,10 @@
       </c>
       <c r="H278">
         <f>VLOOKUP(E278,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I278" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -13922,11 +13926,11 @@
       </c>
       <c r="H279">
         <f>VLOOKUP(E279,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I279" s="5">
-        <f t="shared" si="4"/>
-        <v>-409.12888675238236</v>
+        <f t="shared" si="6"/>
+        <v>263.954120485408</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
@@ -13954,11 +13958,11 @@
       </c>
       <c r="H280">
         <f>VLOOKUP(E280,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I280" s="5">
-        <f t="shared" si="4"/>
-        <v>-326.62764446974836</v>
+        <f t="shared" si="6"/>
+        <v>210.72751256112798</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.25">
@@ -13986,11 +13990,11 @@
       </c>
       <c r="H281">
         <f>VLOOKUP(E281,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I281" s="5">
-        <f t="shared" si="4"/>
-        <v>-0.79856000000000005</v>
+        <f t="shared" si="6"/>
+        <v>0.51519999999999999</v>
       </c>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.25">
@@ -14018,11 +14022,11 @@
       </c>
       <c r="H282">
         <f>VLOOKUP(E282,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="I282" s="5">
-        <f t="shared" si="4"/>
-        <v>-186.08255232839244</v>
+        <f t="shared" si="6"/>
+        <v>120.05325956670481</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.25">
@@ -14050,11 +14054,11 @@
       </c>
       <c r="H283">
         <f>VLOOKUP(E283,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="I283" s="5">
-        <f t="shared" si="4"/>
-        <v>159.02351999999999</v>
+        <f t="shared" si="6"/>
+        <v>365.96160000000003</v>
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.25">
@@ -14082,11 +14086,11 @@
       </c>
       <c r="H284">
         <f>VLOOKUP(E284,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="I284" s="5">
-        <f t="shared" si="4"/>
-        <v>73.742502166666853</v>
+        <f t="shared" si="6"/>
+        <v>169.70397888888931</v>
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.25">
@@ -14114,11 +14118,11 @@
       </c>
       <c r="H285">
         <f>VLOOKUP(E285,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="I285" s="5">
-        <f t="shared" si="4"/>
-        <v>49.678061627451179</v>
+        <f t="shared" si="6"/>
+        <v>114.32436483660176</v>
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.25">
@@ -14149,7 +14153,7 @@
         <v>-1000</v>
       </c>
       <c r="I286" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-51.4413069480673</v>
       </c>
     </row>
@@ -14181,7 +14185,7 @@
         <v>-1000</v>
       </c>
       <c r="I287" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-12943.8875094579</v>
       </c>
     </row>
@@ -14213,7 +14217,7 @@
         <v>-1000</v>
       </c>
       <c r="I288" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-59.347520312196799</v>
       </c>
     </row>
@@ -14245,7 +14249,7 @@
         <v>-1000</v>
       </c>
       <c r="I289" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-104.760537115285</v>
       </c>
     </row>
@@ -14277,7 +14281,7 @@
         <v>-1000</v>
       </c>
       <c r="I290" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-29.609979244837998</v>
       </c>
     </row>
@@ -14309,7 +14313,7 @@
         <v>-1000</v>
       </c>
       <c r="I291" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-9.3910476929126609</v>
       </c>
     </row>
@@ -14341,7 +14345,7 @@
         <v>-1000</v>
       </c>
       <c r="I292" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-455.98754860422702</v>
       </c>
     </row>
@@ -14373,7 +14377,7 @@
         <v>-1000</v>
       </c>
       <c r="I293" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-2230.2147557619701</v>
       </c>
     </row>
@@ -14405,7 +14409,7 @@
         <v>-1000</v>
       </c>
       <c r="I294" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-4941.4070185618093</v>
       </c>
     </row>
@@ -14437,22 +14441,22 @@
         <v>-1000</v>
       </c>
       <c r="I295" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-5618.4556739501995</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I295" xr:uid="{E3C8A208-9E97-4C92-B969-1FB6C28D38FF}"/>
+  <autoFilter ref="A2:I295"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14504,10 +14508,10 @@
       </c>
       <c r="E4">
         <f>F4-(2*(G4+25)*(1+(F4/1000)))</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="F4">
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="G4">
         <v>-25</v>
@@ -14541,13 +14545,13 @@
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E61" si="0">F5-(2*(G5+25)*(1+(F5/1000)))</f>
-        <v>56.3</v>
+        <v>100</v>
       </c>
       <c r="F5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G5">
-        <v>-28</v>
+        <v>-25</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>7</v>
@@ -14567,11 +14571,11 @@
       </c>
       <c r="N5">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L5,naei_ukdata_20210113102859!I:I)</f>
-        <v>-160324.69684390677</v>
+        <v>-147659.21612551695</v>
       </c>
       <c r="O5">
         <f>N5/M5</f>
-        <v>-348.02395829324161</v>
+        <v>-320.53043533593763</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -14591,6 +14595,9 @@
       <c r="F6">
         <v>-1000</v>
       </c>
+      <c r="G6">
+        <v>-25</v>
+      </c>
       <c r="H6" s="3" t="s">
         <v>34</v>
       </c>
@@ -14609,11 +14616,11 @@
       </c>
       <c r="N6">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L6,naei_ukdata_20210113102859!I:I)</f>
-        <v>-67036.71853880315</v>
+        <v>-66090.279521097182</v>
       </c>
       <c r="O6">
         <f t="shared" ref="O6:O14" si="1">N6/M6</f>
-        <v>-792.21076370351136</v>
+        <v>-781.026159305227</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -14633,6 +14640,9 @@
       <c r="F7">
         <v>-1000</v>
       </c>
+      <c r="G7">
+        <v>-25</v>
+      </c>
       <c r="H7" s="3" t="s">
         <v>39</v>
       </c>
@@ -14651,11 +14661,11 @@
       </c>
       <c r="N7">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L7,naei_ukdata_20210113102859!I:I)</f>
-        <v>-168099.50982485997</v>
+        <v>-165920.08301192446</v>
       </c>
       <c r="O7">
         <f t="shared" si="1"/>
-        <v>-796.19380122598204</v>
+        <v>-785.87106964578368</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -14675,6 +14685,9 @@
       <c r="F8">
         <v>-1000</v>
       </c>
+      <c r="G8">
+        <v>-25</v>
+      </c>
       <c r="H8" s="3" t="s">
         <v>52</v>
       </c>
@@ -14712,10 +14725,13 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="F9">
         <v>20</v>
+      </c>
+      <c r="G9">
+        <v>-25</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>56</v>
@@ -14735,11 +14751,11 @@
       </c>
       <c r="N9">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L9,naei_ukdata_20210113102859!I:I)</f>
-        <v>-724.79595417296241</v>
+        <v>1299.8222262848979</v>
       </c>
       <c r="O9">
         <f t="shared" si="1"/>
-        <v>-18.493211427460746</v>
+        <v>33.165040602672896</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -14759,6 +14775,9 @@
       <c r="F10">
         <v>-1000</v>
       </c>
+      <c r="G10">
+        <v>-25</v>
+      </c>
       <c r="H10" s="3" t="s">
         <v>59</v>
       </c>
@@ -14801,6 +14820,9 @@
       <c r="F11">
         <v>-1000</v>
       </c>
+      <c r="G11">
+        <v>-25</v>
+      </c>
       <c r="H11" s="3" t="s">
         <v>61</v>
       </c>
@@ -14819,11 +14841,11 @@
       </c>
       <c r="N11">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L11,naei_ukdata_20210113102859!I:I)</f>
-        <v>-440677.58530559432</v>
+        <v>-423685.48566988361</v>
       </c>
       <c r="O11">
         <f t="shared" si="1"/>
-        <v>-999.99999999999955</v>
+        <v>-961.44097135340462</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -14838,10 +14860,14 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="F12">
-        <v>-1000</v>
+        <f>0.95*-1000+0.05*20</f>
+        <v>-949</v>
+      </c>
+      <c r="G12">
+        <v>-25</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>63</v>
@@ -14861,11 +14887,11 @@
       </c>
       <c r="N12">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L12,naei_ukdata_20210113102859!I:I)</f>
-        <v>-215727.26213003226</v>
+        <v>-204725.17176140059</v>
       </c>
       <c r="O12">
         <f t="shared" si="1"/>
-        <v>-1000.0000000000001</v>
+        <v>-949</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -14885,6 +14911,9 @@
       <c r="F13">
         <v>-1000</v>
       </c>
+      <c r="G13">
+        <v>-25</v>
+      </c>
       <c r="H13" s="3" t="s">
         <v>65</v>
       </c>
@@ -14903,11 +14932,11 @@
       </c>
       <c r="N13">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L13,naei_ukdata_20210113102859!I:I)</f>
-        <v>-129.43452721811903</v>
+        <v>-36.5917796624232</v>
       </c>
       <c r="O13">
         <f t="shared" si="1"/>
-        <v>-68.359212389909189</v>
+        <v>-19.325486726220205</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -14927,6 +14956,9 @@
       <c r="F14">
         <v>-1000</v>
       </c>
+      <c r="G14">
+        <v>-25</v>
+      </c>
       <c r="H14" s="3" t="s">
         <v>69</v>
       </c>
@@ -14945,11 +14977,11 @@
       </c>
       <c r="N14">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L14,naei_ukdata_20210113102859!I:I)</f>
-        <v>-13767.963450136453</v>
+        <v>-12973.283991240372</v>
       </c>
       <c r="O14">
         <f t="shared" si="1"/>
-        <v>-476.94682307485169</v>
+        <v>-449.4177084998438</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -14969,6 +15001,9 @@
       <c r="F15">
         <v>-1000</v>
       </c>
+      <c r="G15">
+        <v>-25</v>
+      </c>
       <c r="H15" s="3" t="s">
         <v>72</v>
       </c>
@@ -15003,6 +15038,9 @@
       <c r="F16">
         <v>-1000</v>
       </c>
+      <c r="G16">
+        <v>-25</v>
+      </c>
       <c r="H16" s="3" t="s">
         <v>77</v>
       </c>
@@ -15031,6 +15069,9 @@
       <c r="F17">
         <v>-1000</v>
       </c>
+      <c r="G17">
+        <v>-25</v>
+      </c>
       <c r="H17" s="3" t="s">
         <v>84</v>
       </c>
@@ -15059,6 +15100,9 @@
       <c r="F18">
         <v>-1000</v>
       </c>
+      <c r="G18">
+        <v>-25</v>
+      </c>
       <c r="H18" s="3" t="s">
         <v>86</v>
       </c>
@@ -15082,10 +15126,13 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="F19">
         <v>20</v>
+      </c>
+      <c r="G19">
+        <v>-25</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>91</v>
@@ -15115,6 +15162,9 @@
       <c r="F20">
         <v>-1000</v>
       </c>
+      <c r="G20">
+        <v>-25</v>
+      </c>
       <c r="H20" s="3" t="s">
         <v>96</v>
       </c>
@@ -15143,6 +15193,9 @@
       <c r="F21">
         <v>-1000</v>
       </c>
+      <c r="G21">
+        <v>-25</v>
+      </c>
       <c r="H21" s="3" t="s">
         <v>106</v>
       </c>
@@ -15166,10 +15219,13 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="F22">
         <v>97</v>
+      </c>
+      <c r="G22">
+        <v>-25</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>113</v>
@@ -15199,6 +15255,9 @@
       <c r="F23">
         <v>-1000</v>
       </c>
+      <c r="G23">
+        <v>-25</v>
+      </c>
       <c r="H23" s="3" t="s">
         <v>118</v>
       </c>
@@ -15227,6 +15286,9 @@
       <c r="F24">
         <v>-1000</v>
       </c>
+      <c r="G24">
+        <v>-25</v>
+      </c>
       <c r="H24" s="3" t="s">
         <v>128</v>
       </c>
@@ -15255,6 +15317,9 @@
       <c r="F25">
         <v>-1000</v>
       </c>
+      <c r="G25">
+        <v>-25</v>
+      </c>
       <c r="H25" s="3" t="s">
         <v>130</v>
       </c>
@@ -15283,6 +15348,9 @@
       <c r="F26">
         <v>-1000</v>
       </c>
+      <c r="G26">
+        <v>-25</v>
+      </c>
       <c r="H26" s="3" t="s">
         <v>132</v>
       </c>
@@ -15306,10 +15374,13 @@
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="F27">
         <v>20</v>
+      </c>
+      <c r="G27">
+        <v>-25</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>137</v>
@@ -15339,6 +15410,9 @@
       <c r="F28">
         <v>-1000</v>
       </c>
+      <c r="G28">
+        <v>-25</v>
+      </c>
       <c r="H28" s="3" t="s">
         <v>139</v>
       </c>
@@ -15362,10 +15436,13 @@
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>59.25</v>
+        <v>115</v>
       </c>
       <c r="F29">
         <v>115</v>
+      </c>
+      <c r="G29">
+        <v>-25</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>142</v>
@@ -15390,10 +15467,13 @@
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="F30">
         <v>97</v>
+      </c>
+      <c r="G30">
+        <v>-25</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>144</v>
@@ -15423,6 +15503,9 @@
       <c r="F31">
         <v>-1000</v>
       </c>
+      <c r="G31">
+        <v>-25</v>
+      </c>
       <c r="H31" s="3" t="s">
         <v>146</v>
       </c>
@@ -15451,6 +15534,9 @@
       <c r="F32">
         <v>-1000</v>
       </c>
+      <c r="G32">
+        <v>-25</v>
+      </c>
       <c r="H32" s="3" t="s">
         <v>149</v>
       </c>
@@ -15474,10 +15560,13 @@
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="F33">
         <v>20</v>
+      </c>
+      <c r="G33">
+        <v>-25</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>156</v>
@@ -15502,10 +15591,13 @@
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>-31</v>
+        <v>20</v>
       </c>
       <c r="F34">
         <v>20</v>
+      </c>
+      <c r="G34">
+        <v>-25</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>161</v>
@@ -15535,6 +15627,9 @@
       <c r="F35">
         <v>-1000</v>
       </c>
+      <c r="G35">
+        <v>-25</v>
+      </c>
       <c r="H35" s="3" t="s">
         <v>164</v>
       </c>
@@ -15563,6 +15658,9 @@
       <c r="F36">
         <v>-1000</v>
       </c>
+      <c r="G36">
+        <v>-25</v>
+      </c>
       <c r="H36" s="3" t="s">
         <v>167</v>
       </c>
@@ -15591,6 +15689,9 @@
       <c r="F37">
         <v>-1000</v>
       </c>
+      <c r="G37">
+        <v>-25</v>
+      </c>
       <c r="H37" s="3" t="s">
         <v>170</v>
       </c>
@@ -15619,6 +15720,9 @@
       <c r="F38">
         <v>-1000</v>
       </c>
+      <c r="G38">
+        <v>-25</v>
+      </c>
       <c r="H38" s="3" t="s">
         <v>174</v>
       </c>
@@ -15647,6 +15751,9 @@
       <c r="F39">
         <v>-1000</v>
       </c>
+      <c r="G39">
+        <v>-25</v>
+      </c>
       <c r="H39" s="3" t="s">
         <v>177</v>
       </c>
@@ -15675,6 +15782,9 @@
       <c r="F40">
         <v>-1000</v>
       </c>
+      <c r="G40">
+        <v>-25</v>
+      </c>
       <c r="H40" s="3" t="s">
         <v>180</v>
       </c>
@@ -15703,6 +15813,9 @@
       <c r="F41">
         <v>-1000</v>
       </c>
+      <c r="G41">
+        <v>-25</v>
+      </c>
       <c r="H41" s="3" t="s">
         <v>186</v>
       </c>
@@ -15731,6 +15844,9 @@
       <c r="F42">
         <v>-1000</v>
       </c>
+      <c r="G42">
+        <v>-25</v>
+      </c>
       <c r="H42" s="3" t="s">
         <v>189</v>
       </c>
@@ -15759,6 +15875,9 @@
       <c r="F43">
         <v>-1000</v>
       </c>
+      <c r="G43">
+        <v>-25</v>
+      </c>
       <c r="H43" s="3" t="s">
         <v>192</v>
       </c>
@@ -15787,6 +15906,9 @@
       <c r="F44">
         <v>-1000</v>
       </c>
+      <c r="G44">
+        <v>-25</v>
+      </c>
       <c r="H44" s="3" t="s">
         <v>195</v>
       </c>
@@ -15815,6 +15937,9 @@
       <c r="F45">
         <v>-1000</v>
       </c>
+      <c r="G45">
+        <v>-25</v>
+      </c>
       <c r="H45" s="3" t="s">
         <v>198</v>
       </c>
@@ -15843,6 +15968,9 @@
       <c r="F46">
         <v>-1000</v>
       </c>
+      <c r="G46">
+        <v>-25</v>
+      </c>
       <c r="H46" s="3" t="s">
         <v>203</v>
       </c>
@@ -15871,6 +15999,9 @@
       <c r="F47">
         <v>-1000</v>
       </c>
+      <c r="G47">
+        <v>-25</v>
+      </c>
       <c r="H47" s="3" t="s">
         <v>209</v>
       </c>
@@ -15899,6 +16030,9 @@
       <c r="F48">
         <v>-1000</v>
       </c>
+      <c r="G48">
+        <v>-25</v>
+      </c>
       <c r="H48" s="3" t="s">
         <v>211</v>
       </c>
@@ -15922,10 +16056,13 @@
       </c>
       <c r="E49">
         <f t="shared" si="0"/>
-        <v>59.25</v>
+        <v>115</v>
       </c>
       <c r="F49">
         <v>115</v>
+      </c>
+      <c r="G49">
+        <v>-25</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>214</v>
@@ -15955,6 +16092,9 @@
       <c r="F50">
         <v>-1000</v>
       </c>
+      <c r="G50">
+        <v>-25</v>
+      </c>
       <c r="H50" s="3" t="s">
         <v>217</v>
       </c>
@@ -15983,6 +16123,9 @@
       <c r="F51">
         <v>-1000</v>
       </c>
+      <c r="G51">
+        <v>-25</v>
+      </c>
       <c r="H51" s="3" t="s">
         <v>220</v>
       </c>
@@ -16006,10 +16149,13 @@
       </c>
       <c r="E52">
         <f t="shared" si="0"/>
-        <v>-1000</v>
+        <v>10</v>
       </c>
       <c r="F52">
-        <v>-1000</v>
+        <v>10</v>
+      </c>
+      <c r="G52">
+        <v>-25</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>230</v>
@@ -16039,6 +16185,9 @@
       <c r="F53">
         <v>-1000</v>
       </c>
+      <c r="G53">
+        <v>-25</v>
+      </c>
       <c r="H53" s="3" t="s">
         <v>233</v>
       </c>
@@ -16067,6 +16216,9 @@
       <c r="F54">
         <v>-1000</v>
       </c>
+      <c r="G54">
+        <v>-25</v>
+      </c>
       <c r="H54" s="3" t="s">
         <v>245</v>
       </c>
@@ -16095,6 +16247,9 @@
       <c r="F55">
         <v>-1000</v>
       </c>
+      <c r="G55">
+        <v>-25</v>
+      </c>
       <c r="H55" s="3" t="s">
         <v>248</v>
       </c>
@@ -16123,6 +16278,9 @@
       <c r="F56">
         <v>-1000</v>
       </c>
+      <c r="G56">
+        <v>-25</v>
+      </c>
       <c r="H56" s="3" t="s">
         <v>251</v>
       </c>
@@ -16151,6 +16309,9 @@
       <c r="F57">
         <v>-1000</v>
       </c>
+      <c r="G57">
+        <v>-25</v>
+      </c>
       <c r="H57" s="3" t="s">
         <v>256</v>
       </c>
@@ -16179,6 +16340,9 @@
       <c r="F58">
         <v>-1000</v>
       </c>
+      <c r="G58">
+        <v>-25</v>
+      </c>
       <c r="H58" s="3" t="s">
         <v>258</v>
       </c>
@@ -16207,6 +16371,9 @@
       <c r="F59">
         <v>-1000</v>
       </c>
+      <c r="G59">
+        <v>-25</v>
+      </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
@@ -16225,6 +16392,9 @@
       <c r="F60">
         <v>-1000</v>
       </c>
+      <c r="G60">
+        <v>-25</v>
+      </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
@@ -16243,6 +16413,9 @@
       <c r="F61">
         <v>-1000</v>
       </c>
+      <c r="G61">
+        <v>-25</v>
+      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -16254,6 +16427,9 @@
       <c r="D62" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="G62">
+        <v>-25</v>
+      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
@@ -16265,6 +16441,9 @@
       <c r="D63" s="3" t="s">
         <v>207</v>
       </c>
+      <c r="G63">
+        <v>-25</v>
+      </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
@@ -16276,8 +16455,11 @@
       <c r="D64" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>205</v>
       </c>
@@ -16287,8 +16469,11 @@
       <c r="D65" s="3" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>25</v>
       </c>
@@ -16298,8 +16483,11 @@
       <c r="D66" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>229</v>
       </c>
@@ -16309,8 +16497,11 @@
       <c r="D67" s="3" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>226</v>
       </c>
@@ -16320,8 +16511,11 @@
       <c r="D68" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>26</v>
       </c>
@@ -16331,8 +16525,11 @@
       <c r="D69" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>27</v>
       </c>
@@ -16342,8 +16539,11 @@
       <c r="D70" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>141</v>
       </c>
@@ -16353,8 +16553,11 @@
       <c r="D71" s="3" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>206</v>
       </c>
@@ -16364,8 +16567,11 @@
       <c r="D72" s="3" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>225</v>
       </c>
@@ -16375,8 +16581,11 @@
       <c r="D73" s="3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>208</v>
       </c>
@@ -16386,8 +16595,11 @@
       <c r="D74" s="3" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>21</v>
       </c>
@@ -16397,8 +16609,11 @@
       <c r="D75" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>228</v>
       </c>
@@ -16408,8 +16623,11 @@
       <c r="D76" s="3" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>36</v>
       </c>
@@ -16419,8 +16637,11 @@
       <c r="D77" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>261</v>
       </c>
@@ -16434,7 +16655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D4F4FA-89CA-4DF2-92B9-60EBA76C9E3D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16474,7 +16695,7 @@
       </c>
       <c r="C2">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A2,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A2,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-669.48231862687817</v>
+        <v>-651.69164968422979</v>
       </c>
       <c r="D2">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A2,naei_ukdata_20210113102859!G:G)</f>
@@ -16482,7 +16703,7 @@
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>-35615.534753378124</v>
+        <v>-34669.095735672156</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -16663,7 +16884,7 @@
       </c>
       <c r="C11">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A11,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A11,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-1000</v>
+        <v>-953.64706414246155</v>
       </c>
       <c r="D11">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A11,naei_ukdata_20210113102859!G:G)</f>
@@ -16671,7 +16892,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>-245468.10539847688</v>
+        <v>-234089.93805386982</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -16684,7 +16905,7 @@
       </c>
       <c r="C12">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A12,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A12,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-395.93393708391022</v>
+        <v>-365.33814627038328</v>
       </c>
       <c r="D12">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A12,naei_ukdata_20210113102859!G:G)</f>
@@ -16692,7 +16913,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>-28203.521323929152</v>
+        <v>-26024.094510993673</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -16747,7 +16968,7 @@
       </c>
       <c r="C15">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A15,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A15,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-1000.0000000000002</v>
+        <v>-948.99999999999989</v>
       </c>
       <c r="D15">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A15,naei_ukdata_20210113102859!G:G)</f>
@@ -16755,7 +16976,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>-179714.38754564128</v>
+        <v>-170548.95378081352</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -16768,7 +16989,7 @@
       </c>
       <c r="C16">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A16,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A16,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-999.99999999999977</v>
+        <v>-948.99999999999977</v>
       </c>
       <c r="D16">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A16,naei_ukdata_20210113102859!G:G)</f>
@@ -16776,7 +16997,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>-12757.108996950825</v>
+        <v>-12106.496438106333</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -16789,7 +17010,7 @@
       </c>
       <c r="C17">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A17,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A17,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-1000.0000000000002</v>
+        <v>-949.00000000000011</v>
       </c>
       <c r="D17">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A17,naei_ukdata_20210113102859!G:G)</f>
@@ -16797,7 +17018,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>-12879.28961522902</v>
+        <v>-12222.445844852338</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -16810,7 +17031,7 @@
       </c>
       <c r="C18">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A18,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A18,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-999.99999999999989</v>
+        <v>-948.99999999999989</v>
       </c>
       <c r="D18">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A18,naei_ukdata_20210113102859!G:G)</f>
@@ -16818,7 +17039,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>-10376.475972211158</v>
+        <v>-9847.275697628389</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -16852,7 +17073,7 @@
       </c>
       <c r="C20">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A20,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A20,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-1000</v>
+        <v>-955.08435323502999</v>
       </c>
       <c r="D20">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A20,naei_ukdata_20210113102859!G:G)</f>
@@ -16860,7 +17081,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>-41192.099482468686</v>
+        <v>-39341.929692606616</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -16915,7 +17136,7 @@
       </c>
       <c r="C23">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A23,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A23,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-332.61921953015138</v>
+        <v>-304.52544592954877</v>
       </c>
       <c r="D23">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A23,naei_ukdata_20210113102859!G:G)</f>
@@ -16923,7 +17144,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>-148640.49922085821</v>
+        <v>-136085.98556740768</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -16936,7 +17157,7 @@
       </c>
       <c r="C24">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A24,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A24,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-1000</v>
+        <v>-949</v>
       </c>
       <c r="D24">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A24,naei_ukdata_20210113102859!G:G)</f>
@@ -16944,7 +17165,7 @@
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>-72722.618045667434</v>
+        <v>-69013.764525338396</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -16957,7 +17178,7 @@
       </c>
       <c r="C25">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A25,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A25,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-99.843897140822008</v>
+        <v>-52.467260148233684</v>
       </c>
       <c r="D25">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A25,naei_ukdata_20210113102859!G:G)</f>
@@ -16965,7 +17186,7 @@
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>-233.8575492293962</v>
+        <v>-122.8904842901055</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -16978,7 +17199,7 @@
       </c>
       <c r="C26">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A26,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A26,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-1000.0000000000001</v>
+        <v>-997.72965654194854</v>
       </c>
       <c r="D26">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A26,naei_ukdata_20210113102859!G:G)</f>
@@ -16986,7 +17207,7 @@
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>-24185.319061695522</v>
+        <v>-24130.410080782913</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -17314,7 +17535,7 @@
       </c>
       <c r="C42">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A42,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A42,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-68.359212389909189</v>
+        <v>-19.325486726220205</v>
       </c>
       <c r="D42">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A42,naei_ukdata_20210113102859!G:G)</f>
@@ -17322,7 +17543,7 @@
       </c>
       <c r="E42">
         <f t="shared" si="0"/>
-        <v>-129.43452721811903</v>
+        <v>-36.5917796624232</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -17461,7 +17682,7 @@
       </c>
       <c r="C49">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A49,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A49,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>59.25</v>
+        <v>115</v>
       </c>
       <c r="D49">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A49,naei_ukdata_20210113102859!G:G)</f>
@@ -17469,7 +17690,7 @@
       </c>
       <c r="E49">
         <f t="shared" si="0"/>
-        <v>339.46981694964319</v>
+        <v>658.88656454361126</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -17482,7 +17703,7 @@
       </c>
       <c r="C50">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A50,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A50,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>42.15</v>
+        <v>97.000000000000028</v>
       </c>
       <c r="D50">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A50,naei_ukdata_20210113102859!G:G)</f>
@@ -17490,7 +17711,7 @@
       </c>
       <c r="E50">
         <f t="shared" si="0"/>
-        <v>365.22011451930535</v>
+        <v>840.48282582141485</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -17503,7 +17724,7 @@
       </c>
       <c r="C51">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A51,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A51,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-31</v>
+        <v>20.000000000000004</v>
       </c>
       <c r="D51">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A51,naei_ukdata_20210113102859!G:G)</f>
@@ -17511,7 +17732,7 @@
       </c>
       <c r="E51">
         <f t="shared" si="0"/>
-        <v>-1007.2400379670804</v>
+        <v>649.83228255940685</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -17524,7 +17745,7 @@
       </c>
       <c r="C52">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A52,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A52,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>42.15</v>
+        <v>97</v>
       </c>
       <c r="D52">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A52,naei_ukdata_20210113102859!G:G)</f>
@@ -17532,7 +17753,7 @@
       </c>
       <c r="E52">
         <f t="shared" si="0"/>
-        <v>159.02351999999999</v>
+        <v>365.96160000000003</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -17545,7 +17766,7 @@
       </c>
       <c r="C53">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A53,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A53,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>42.150000000000006</v>
+        <v>97.000000000000014</v>
       </c>
       <c r="D53">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A53,naei_ukdata_20210113102859!G:G)</f>
@@ -17553,7 +17774,7 @@
       </c>
       <c r="E53">
         <f t="shared" si="0"/>
-        <v>123.42056379411804</v>
+        <v>284.02834372549108</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -17625,11 +17846,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17652,7 +17873,7 @@
       </c>
       <c r="B3">
         <f>SUMIF(Sheet3!B:B,Sheet2!A3,Sheet3!E:E)/SUMIF(Sheet3!B:B,Sheet2!A3,Sheet3!D:D)</f>
-        <v>-348.02395829324166</v>
+        <v>-320.53043533593768</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -17669,7 +17890,7 @@
       </c>
       <c r="B5">
         <f>SUMIF(Sheet3!B:B,Sheet2!A5,Sheet3!E:E)/SUMIF(Sheet3!B:B,Sheet2!A5,Sheet3!D:D)</f>
-        <v>-796.19380122598238</v>
+        <v>-785.87106964578402</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -17687,7 +17908,7 @@
       </c>
       <c r="B7">
         <f>SUMIF(Sheet3!B:B,Sheet2!A7,Sheet3!E:E)/SUMIF(Sheet3!B:B,Sheet2!A7,Sheet3!D:D)</f>
-        <v>-18.493211427460746</v>
+        <v>33.165040602672903</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -17705,7 +17926,7 @@
       </c>
       <c r="B9">
         <f>SUMIF(Sheet3!B:B,Sheet2!A9,Sheet3!E:E)/SUMIF(Sheet3!B:B,Sheet2!A9,Sheet3!D:D)</f>
-        <v>-999.99999999999989</v>
+        <v>-961.44097135340473</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -17714,7 +17935,7 @@
       </c>
       <c r="B10">
         <f>SUMIF(Sheet3!B:B,Sheet2!A10,Sheet3!E:E)/SUMIF(Sheet3!B:B,Sheet2!A10,Sheet3!D:D)</f>
-        <v>-1000.0000000000002</v>
+        <v>-948.99999999999977</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -17723,7 +17944,7 @@
       </c>
       <c r="B11">
         <f>SUMIF(Sheet3!B:B,Sheet2!A11,Sheet3!E:E)/SUMIF(Sheet3!B:B,Sheet2!A11,Sheet3!D:D)</f>
-        <v>-68.359212389909189</v>
+        <v>-19.325486726220205</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -17732,7 +17953,7 @@
       </c>
       <c r="B12">
         <f>SUMIF(Sheet3!B:B,Sheet2!A12,Sheet3!E:E)/SUMIF(Sheet3!B:B,Sheet2!A12,Sheet3!D:D)</f>
-        <v>-476.94682307485169</v>
+        <v>-449.41770849984385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committed changes to several files
</commit_message>
<xml_diff>
--- a/Distribution calcs.xlsx
+++ b/Distribution calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="naei_ukdata_20210113102859" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="9" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -4270,7 +4270,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B78" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -4616,7 +4616,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L4:M15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -4983,7 +4983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J295"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
@@ -5531,11 +5531,11 @@
       </c>
       <c r="H18">
         <f>VLOOKUP(E18,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" si="0"/>
-        <v>918.1728145065041</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -8602,11 +8602,11 @@
       </c>
       <c r="H114">
         <f>VLOOKUP(E114,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I114" s="5">
         <f t="shared" si="1"/>
-        <v>716.93192099999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -11802,11 +11802,11 @@
       </c>
       <c r="H213">
         <f>VLOOKUP(E213,'Distribution calcs'!D:E,2,FALSE)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I213" s="5">
         <f t="shared" si="3"/>
-        <v>26417.082355390499</v>
+        <v>0</v>
       </c>
       <c r="J213">
         <f>G213/SUMIF(C:C,C$186,G:G)</f>
@@ -14455,8 +14455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O78"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14544,8 +14544,7 @@
         <v>24</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E61" si="0">F5-(2*(G5+25)*(1+(F5/1000)))</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -14571,11 +14570,11 @@
       </c>
       <c r="N5">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L5,naei_ukdata_20210113102859!I:I)</f>
-        <v>-147659.21612551695</v>
+        <v>-174076.29848090746</v>
       </c>
       <c r="O5">
         <f>N5/M5</f>
-        <v>-320.53043533593763</v>
+        <v>-377.87517229079793</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -14589,7 +14588,7 @@
         <v>14</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E5:E61" si="0">F6-(2*(G6+25)*(1+(F6/1000)))</f>
         <v>-1000</v>
       </c>
       <c r="F6">
@@ -14616,11 +14615,11 @@
       </c>
       <c r="N6">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L6,naei_ukdata_20210113102859!I:I)</f>
-        <v>-66090.279521097182</v>
+        <v>-67008.452335603681</v>
       </c>
       <c r="O6">
         <f t="shared" ref="O6:O14" si="1">N6/M6</f>
-        <v>-781.026159305227</v>
+        <v>-791.87672601622978</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -14661,11 +14660,11 @@
       </c>
       <c r="N7">
         <f>SUMIF(naei_ukdata_20210113102859!C:C,'Distribution calcs'!L7,naei_ukdata_20210113102859!I:I)</f>
-        <v>-165920.08301192446</v>
+        <v>-166637.01493292447</v>
       </c>
       <c r="O7">
         <f t="shared" si="1"/>
-        <v>-785.87106964578368</v>
+        <v>-789.26677705739939</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -16695,7 +16694,7 @@
       </c>
       <c r="C2">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A2,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A2,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-651.69164968422979</v>
+        <v>-668.95098522453588</v>
       </c>
       <c r="D2">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A2,naei_ukdata_20210113102859!G:G)</f>
@@ -16703,7 +16702,7 @@
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>-34669.095735672156</v>
+        <v>-35587.268550178662</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -16905,7 +16904,7 @@
       </c>
       <c r="C12">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A12,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A12,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-365.33814627038328</v>
+        <v>-375.40276461510831</v>
       </c>
       <c r="D12">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A12,naei_ukdata_20210113102859!G:G)</f>
@@ -16913,7 +16912,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>-26024.094510993673</v>
+        <v>-26741.026431993672</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -17136,7 +17135,7 @@
       </c>
       <c r="C23">
         <f>IFERROR(SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A23,naei_ukdata_20210113102859!I:I)/SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A23,naei_ukdata_20210113102859!G:G),0)</f>
-        <v>-304.52544592954877</v>
+        <v>-363.64008400848695</v>
       </c>
       <c r="D23">
         <f>SUMIF(naei_ukdata_20210113102859!B:B,Sheet3!A23,naei_ukdata_20210113102859!G:G)</f>
@@ -17144,7 +17143,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>-136085.98556740768</v>
+        <v>-162503.06792279819</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -17873,7 +17872,7 @@
       </c>
       <c r="B3">
         <f>SUMIF(Sheet3!B:B,Sheet2!A3,Sheet3!E:E)/SUMIF(Sheet3!B:B,Sheet2!A3,Sheet3!D:D)</f>
-        <v>-320.53043533593768</v>
+        <v>-377.87517229079799</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -17890,7 +17889,7 @@
       </c>
       <c r="B5">
         <f>SUMIF(Sheet3!B:B,Sheet2!A5,Sheet3!E:E)/SUMIF(Sheet3!B:B,Sheet2!A5,Sheet3!D:D)</f>
-        <v>-785.87106964578402</v>
+        <v>-789.26677705739974</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>